<commit_message>
Updates for renal validation.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/RenalValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/RenalValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_documentation\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E74A66-7B4C-48DC-918B-0EAB832275AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC7C0EE-62AE-4DCF-AEB8-617BD92526A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25005" yWindow="5820" windowWidth="29955" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23685" yWindow="3825" windowWidth="32160" windowHeight="23445" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -19,13 +19,13 @@
     <sheet name="HemorrhageClass2NoFluid" sheetId="5" r:id="rId4"/>
     <sheet name="HemorrhageClass3NoFluid" sheetId="6" r:id="rId5"/>
     <sheet name="HighAltitudeEnvironmentChange" sheetId="7" r:id="rId6"/>
-    <sheet name="SalineIngestion" sheetId="1" r:id="rId7"/>
+    <sheet name="SodiumIngestion" sheetId="1" r:id="rId7"/>
     <sheet name="WaterIngestion" sheetId="8" r:id="rId8"/>
     <sheet name="Starvation (Removed)" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">BilateralStenosis!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">SalineIngestion!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">SodiumIngestion!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">UnilateralStenosis!#REF!</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="87">
   <si>
     <t>Action</t>
   </si>
@@ -94,12 +94,6 @@
     <t>Stop Hemorrhage</t>
   </si>
   <si>
-    <t>Urine Chloride Concentration (g/L)</t>
-  </si>
-  <si>
-    <t>Urine Urea Concentration (g/L)</t>
-  </si>
-  <si>
     <t>Initiate Environment Change</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>After stabilization patient given 1L of water</t>
   </si>
   <si>
-    <t>Urine sodium concentration (mg/L)</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -232,9 +223,6 @@
     <t>Increased Then Normal @cite dean1949renal</t>
   </si>
   <si>
-    <t>&lt;/span&gt;|&lt;span class="Warning"&gt;</t>
-  </si>
-  <si>
     <t>Plasma Sodium Concentration (mg/L)</t>
   </si>
   <si>
@@ -308,6 +296,15 @@
   </si>
   <si>
     <t>Patient ingests 1 L of water</t>
+  </si>
+  <si>
+    <t>Bladder sodium concentration (mg/L)</t>
+  </si>
+  <si>
+    <t>Bladder Chloride Concentration (g/L)</t>
+  </si>
+  <si>
+    <t>Bladder Urea Concentration (g/L)</t>
   </si>
 </sst>
 </file>
@@ -538,7 +535,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -609,8 +606,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -957,7 +963,7 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
@@ -978,353 +984,353 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F3" s="20">
         <v>7</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H3" s="21">
         <v>1</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J3" s="22">
         <v>0</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F4" s="20">
         <v>7</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H4" s="21">
         <v>1</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J4" s="22">
         <v>0</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F5" s="20">
         <v>8</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H5" s="21">
         <v>0</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J5" s="22">
         <v>0</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F6" s="20">
         <v>8</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H6" s="21">
         <v>0</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J6" s="22">
         <v>0</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F7" s="20">
         <v>3</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H7" s="21">
         <v>0</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J7" s="22">
         <v>0</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F8" s="20">
         <v>1</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H8" s="21">
         <v>1</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J8" s="22">
         <v>0</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F9" s="20">
         <v>1</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H9" s="21">
         <v>3</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J9" s="22">
         <v>0</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10" s="20">
         <f>SUM(F3:F9)</f>
         <v>35</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H10" s="21">
         <f>SUM(H3:H9)</f>
         <v>6</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J10" s="22">
         <f>SUM(J3:J9)</f>
         <v>0</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1383,215 +1389,215 @@
   <sheetData>
     <row r="1" spans="2:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:24" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3">
         <v>120</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="X3" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1643,215 +1649,215 @@
   <sheetData>
     <row r="1" spans="2:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:24" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3">
         <v>120</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="V3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="X3" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1895,210 +1901,210 @@
   <sheetData>
     <row r="1" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5">
         <v>30</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I3" s="5">
         <v>600</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="3">
         <v>620</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3">
         <v>1000</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2137,210 +2143,210 @@
   <sheetData>
     <row r="1" spans="2:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:18" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5">
         <v>30</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I3" s="5">
         <v>600</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="3">
         <v>605</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3">
         <v>1000</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="R4" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2378,141 +2384,141 @@
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G6" s="3">
         <v>50</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I6" s="3">
         <v>900</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2525,10 +2531,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:P4"/>
+  <dimension ref="B2:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2536,158 +2542,177 @@
     <col min="2" max="2" width="2.5703125" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="33.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="38.28515625" customWidth="1"/>
-    <col min="12" max="12" width="24.85546875" customWidth="1"/>
-    <col min="13" max="13" width="36.85546875" customWidth="1"/>
-    <col min="14" max="14" width="30.5703125" customWidth="1"/>
-    <col min="15" max="15" width="31.5703125" customWidth="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="38.28515625" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" customWidth="1"/>
+    <col min="15" max="15" width="36.85546875" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="17" max="17" width="31.5703125" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="10" t="s">
+    <row r="2" spans="2:18" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3600</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="N4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>30</v>
+      <c r="P4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2702,10 +2727,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B1:R4"/>
+  <dimension ref="B2:R4"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2717,173 +2742,172 @@
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
     <col min="10" max="10" width="25.140625" customWidth="1"/>
     <col min="11" max="11" width="31.5703125" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
     <col min="13" max="13" width="31.85546875" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" customWidth="1"/>
     <col min="15" max="15" width="30.140625" customWidth="1"/>
-    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
     <col min="17" max="17" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:18" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="10" t="s">
+    <row r="2" spans="2:18" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="10" t="s">
+      <c r="F2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>23</v>
+      <c r="N2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>23</v>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3">
+        <v>21</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5">
         <v>0</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="3">
-        <v>14400</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="H4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3600</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>30</v>
+      <c r="K4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2922,159 +2946,159 @@
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="R2" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3">
         <v>4</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="25" t="s">
-        <v>69</v>
+        <v>43</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>